<commit_message>
AFDP-6836 FOIA - Fundamental FOIA Changes - Request Created vs. Received Date
</commit_message>
<xml_diff>
--- a/acm-standard-applications/acm-foia/src/main/resources/rules/drools-assignment-rules-foia.xlsx
+++ b/acm-standard-applications/acm-foia/src/main/resources/rules/drools-assignment-rules-foia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller\dev\foia-extension\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C82E0C9-7E7C-4A17-8F6D-153065BCB700}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,22 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
   <si>
     <t>RuleSet</t>
   </si>
@@ -58,129 +69,6 @@
   </si>
   <si>
     <t>Functions</t>
-  </si>
-  <si>
-    <t>Sequential</t>
-  </si>
-  <si>
-    <t>RuleTable Assignment Rules</t>
-  </si>
-  <si>
-    <t>CONDITION</t>
-  </si>
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>$acmObject: AcmAssignedObject</t>
-  </si>
-  <si>
-    <t>objectType.equals("$param")</t>
-  </si>
-  <si>
-    <t>addParticipant($acmObject, "$1", "$2");</t>
-  </si>
-  <si>
-    <t>If different rules apply to the same object, all rules apply; changes made by subsequent rules overwrite changes made by previous rules.</t>
-  </si>
-  <si>
-    <t>Rule Name</t>
-  </si>
-  <si>
-    <t>Type of Object to be Assigned</t>
-  </si>
-  <si>
-    <t>Expression 1
-Must be a Spring expression that evaluates to true or false.</t>
-  </si>
-  <si>
-    <t>Expression 2
-Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
-  </si>
-  <si>
-    <t>Expression 3
-Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
-  </si>
-  <si>
-    <t>COMPLAINT</t>
-  </si>
-  <si>
-    <t>status == 'DRAFT'</t>
-  </si>
-  <si>
-    <t>Complaint – Default access</t>
-  </si>
-  <si>
-    <t>participants.?[participantType == '*'].isEmpty()</t>
-  </si>
-  <si>
-    <t>*, *</t>
-  </si>
-  <si>
-    <t>CASE_FILE</t>
-  </si>
-  <si>
-    <t>Case File – Default access</t>
-  </si>
-  <si>
-    <t>Complaint – Default group</t>
-  </si>
-  <si>
-    <t>participants.?[participantType == 'owning group'].isEmpty()</t>
-  </si>
-  <si>
-    <t>Case File – Default group</t>
-  </si>
-  <si>
-    <t>Folder – default access</t>
-  </si>
-  <si>
-    <t>FOLDER</t>
-  </si>
-  <si>
-    <t>Object Types</t>
-  </si>
-  <si>
-    <t>Participant Types</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>TASK</t>
-  </si>
-  <si>
-    <t>Owner's Supervisor</t>
-  </si>
-  <si>
-    <t>FILE</t>
-  </si>
-  <si>
-    <t>PARTICIPANT</t>
-  </si>
-  <si>
-    <t>ACCESS CONTROL LIST</t>
-  </si>
-  <si>
-    <t>Case File - creator read access</t>
-  </si>
-  <si>
-    <t>eval(evalBoolean("$param", $acmObject))</t>
-  </si>
-  <si>
-    <t>reader, creator</t>
-  </si>
-  <si>
-    <t>EscapeQuotes</t>
-  </si>
-  <si>
-    <t>Assign a literal participant.  First value must be the participant type, second value must be the participant LDAP ID.</t>
-  </si>
-  <si>
-    <t>addParticipantExpression($acmObject, "$1", "$2");</t>
-  </si>
-  <si>
-    <t>Assign a participant.  First value must be the participant type, second value must be an SpEL expression that is valid when evaluated against the $acmObject.</t>
   </si>
   <si>
     <t>function Boolean evalBoolean(String expression, Object obj)
@@ -197,48 +85,243 @@
     Expression exp = ep.parseExpression(expression);
     EvaluationContext ec = new StandardEvaluationContext();
     String evaluated = exp.getValue(ec, obj, String.class);
-    boolean found = false;
-    for ( AcmParticipant ap : obj.getParticipants() )
-    {
-       if ( ap.getParticipantLdapId().equals(evaluated) &amp;&amp; ap.getParticipantType().equals(participantType) )
-      {
-        found = true;
-        break;
-      }
-    }
-    if (!found) 
-    {
-     addParticipant(obj, participantType, evaluated);
-    }
+    addParticipant(obj, participantType, evaluated);
 }
 function void addParticipant(AcmAssignedObject obj, String participantType, String participantId)
 {
+    for ( AcmParticipant ap : obj.getParticipants() )
+    {
+       if ( ap.getParticipantLdapId().equals(participantId) &amp;&amp; ap.getParticipantType().equals(participantType) )
+      {
+        return;
+      }
+    }
     AcmParticipant ap = new AcmParticipant();
     ap.setParticipantType(participantType);
     ap.setParticipantLdapId(participantId);
+    ap.setReplaceChildrenParticipant(true); 
     obj.getParticipants().add(ap);
 }</t>
   </si>
   <si>
-    <t>owning group, ACM_ADMINISTRATOR_DEV</t>
+    <t>EscapeQuotes</t>
+  </si>
+  <si>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>RuleTable Assignment Rules</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>$acmObject: AcmAssignedObject</t>
+  </si>
+  <si>
+    <t>objectType.equals("$param")</t>
+  </si>
+  <si>
+    <t>eval(evalBoolean("$param", $acmObject))</t>
+  </si>
+  <si>
+    <t>addParticipant($acmObject, "$1", "$2");</t>
+  </si>
+  <si>
+    <t>addParticipantExpression($acmObject, "$1", "$2");</t>
+  </si>
+  <si>
+    <t>If different rules apply to the same object, all rules apply; changes made by subsequent rules overwrite changes made by previous rules.</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>Type of Object to be Assigned</t>
+  </si>
+  <si>
+    <t>Expression 1
+Must be a Spring expression that evaluates to true or false.</t>
+  </si>
+  <si>
+    <t>Expression 2
+Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
+  </si>
+  <si>
+    <t>Expression 3
+Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
+  </si>
+  <si>
+    <t>Assign a literal participant.  First value must be the participant type, second value must be the participant LDAP ID.</t>
+  </si>
+  <si>
+    <t>Assign a participant.  First value must be the participant type, second value must be an SpEL expression that is valid when evaluated against the $acmObject.</t>
+  </si>
+  <si>
+    <t>Complaint – Default assignee</t>
+  </si>
+  <si>
+    <t>COMPLAINT</t>
+  </si>
+  <si>
+    <t>status == 'DRAFT'</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == 'assignee'].isEmpty()</t>
+  </si>
+  <si>
+    <t>assignee, new String('')</t>
+  </si>
+  <si>
+    <t>Complaint – Default access</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == '*'].isEmpty()</t>
+  </si>
+  <si>
+    <t>*, *</t>
   </si>
   <si>
     <t>Case File – Default assignee</t>
   </si>
   <si>
-    <t>participants.?[participantType == 'assignee'].isEmpty()</t>
-  </si>
-  <si>
-    <t>assignee, new String('')</t>
-  </si>
-  <si>
-    <t>Complaint – Default assignee</t>
+    <t>CASE_FILE</t>
+  </si>
+  <si>
+    <t>Case File – Default access</t>
+  </si>
+  <si>
+    <t>Complaint – Default group</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == 'owning group'].isEmpty()</t>
+  </si>
+  <si>
+    <t>owning group, ARKCASE_ADMINISTRATOR@ARMEDIA.COM</t>
+  </si>
+  <si>
+    <t>Case File – Default group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owning group, OFFICERS@ARMEDIA.COM
+</t>
+  </si>
+  <si>
+    <t>File - default access</t>
+  </si>
+  <si>
+    <t>FILE</t>
+  </si>
+  <si>
+    <t>Folder – default access</t>
+  </si>
+  <si>
+    <t>FOLDER</t>
+  </si>
+  <si>
+    <t>Case File - creator read access</t>
+  </si>
+  <si>
+    <t>reader, creator</t>
+  </si>
+  <si>
+    <t>Complaint - creator read access</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Default access</t>
+  </si>
+  <si>
+    <t>DOC_REPO</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Default group</t>
+  </si>
+  <si>
+    <t>owning group, ARKCASE_SUPERVISOR@ARMEDIA.COM</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Default owner</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == 'owner'].isEmpty()</t>
+  </si>
+  <si>
+    <t>creator != null</t>
+  </si>
+  <si>
+    <t>owner, creator</t>
+  </si>
+  <si>
+    <t>Organization – Default access</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Organization – Default owner</t>
+  </si>
+  <si>
+    <t>Organization – Default group</t>
+  </si>
+  <si>
+    <t>owning group, ARKCASE_ENTITY_ADMINISTRATOR@ARMEDIA.COM</t>
+  </si>
+  <si>
+    <t>Person – Default access</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>Person – Default owner</t>
+  </si>
+  <si>
+    <t>Person – Default group</t>
+  </si>
+  <si>
+    <t>Costsheet – Default access</t>
+  </si>
+  <si>
+    <t>COSTSHEET</t>
+  </si>
+  <si>
+    <t>Costsheet - creator read access</t>
+  </si>
+  <si>
+    <t>Costsheet – Default owner</t>
+  </si>
+  <si>
+    <t>Object Types</t>
+  </si>
+  <si>
+    <t>Participant Types</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>Owner's Supervisor</t>
+  </si>
+  <si>
+    <t>PARTICIPANT</t>
+  </si>
+  <si>
+    <t>ACCESS CONTROL LIST</t>
+  </si>
+  <si>
+    <t>assignee, owen.officer@armedia.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -479,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -513,7 +596,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +698,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -628,7 +710,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -895,30 +977,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875"/>
-    <col min="2" max="2" width="24.36328125"/>
-    <col min="3" max="3" width="49.90625"/>
-    <col min="4" max="4" width="81.81640625" customWidth="1"/>
-    <col min="5" max="5" width="43.90625"/>
-    <col min="6" max="6" width="30.54296875"/>
-    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.6328125"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -928,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -938,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -948,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -958,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -968,7 +1050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -978,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -988,7 +1070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -998,42 +1080,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="21" t="b">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" s="8" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1041,33 +1124,33 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1075,208 +1158,455 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G21" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>24</v>
-      </c>
       <c r="D23" s="18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="19" t="s">
-        <v>52</v>
+      <c r="G24" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
-        <v>46</v>
+      <c r="G26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="19"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1286,60 +1616,60 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125"/>
-    <col min="2" max="2" width="17.54296875"/>
-    <col min="3" max="1025" width="8.6328125"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1347,12 +1677,12 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.6328125"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>